<commit_message>
update example file for exploded output
</commit_message>
<xml_diff>
--- a/example_output_files/annotated_example_CaC-exploded.xlsx
+++ b/example_output_files/annotated_example_CaC-exploded.xlsx
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P7"/>
+  <dimension ref="A1:Q7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -452,32 +452,32 @@
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>Crisis-A-11_S11_L001</t>
+          <t>Crisis-A</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>Crisis-B-14_S14_L001</t>
+          <t>Crisis-B</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>Crisis-C-17_S17_L001</t>
+          <t>Crisis-C</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>Pre-A-2_S2_L001</t>
+          <t>Pre-A</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>Pre-B-5_S5_L001</t>
+          <t>Pre-B</t>
         </is>
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
-          <t>Pre-C-8_S8_L001</t>
+          <t>Pre-C</t>
         </is>
       </c>
       <c r="J1" s="1" t="inlineStr">
@@ -487,30 +487,35 @@
       </c>
       <c r="K1" s="1" t="inlineStr">
         <is>
-          <t>repeats</t>
+          <t>reg-cen_distance</t>
         </is>
       </c>
       <c r="L1" s="1" t="inlineStr">
         <is>
+          <t>censat_repeats</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
           <t>fragile_sites</t>
         </is>
       </c>
-      <c r="M1" s="1" t="inlineStr">
+      <c r="N1" s="1" t="inlineStr">
         <is>
           <t>genes</t>
         </is>
       </c>
-      <c r="N1" s="1" t="inlineStr">
+      <c r="O1" s="1" t="inlineStr">
         <is>
           <t>gene_lengths</t>
         </is>
       </c>
-      <c r="O1" s="1" t="inlineStr">
+      <c r="P1" s="1" t="inlineStr">
         <is>
           <t>gene-telomere_distances</t>
         </is>
       </c>
-      <c r="P1" s="1" t="inlineStr">
+      <c r="Q1" s="1" t="inlineStr">
         <is>
           <t>gene_positions</t>
         </is>
@@ -567,28 +572,33 @@
           <t>143369</t>
         </is>
       </c>
-      <c r="K2" t="inlineStr"/>
-      <c r="L2" t="inlineStr">
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>121649679</t>
+        </is>
+      </c>
+      <c r="L2" t="inlineStr"/>
+      <c r="M2" t="inlineStr">
         <is>
           <t>FRA1A</t>
         </is>
       </c>
-      <c r="M2" t="inlineStr">
+      <c r="N2" t="inlineStr">
         <is>
           <t>SEPTIN14P22</t>
         </is>
       </c>
-      <c r="N2" t="inlineStr">
+      <c r="O2" t="inlineStr">
         <is>
           <t>2583</t>
         </is>
       </c>
-      <c r="O2" t="inlineStr">
+      <c r="P2" t="inlineStr">
         <is>
           <t>141134</t>
         </is>
       </c>
-      <c r="P2" t="inlineStr">
+      <c r="Q2" t="inlineStr">
         <is>
           <t>chr1:144134-146717</t>
         </is>
@@ -645,28 +655,33 @@
           <t>143369</t>
         </is>
       </c>
-      <c r="K3" t="inlineStr"/>
-      <c r="L3" t="inlineStr">
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>121649679</t>
+        </is>
+      </c>
+      <c r="L3" t="inlineStr"/>
+      <c r="M3" t="inlineStr">
         <is>
           <t>FRA1A</t>
         </is>
       </c>
-      <c r="M3" t="inlineStr">
+      <c r="N3" t="inlineStr">
         <is>
           <t>SEPTIN14P13</t>
         </is>
       </c>
-      <c r="N3" t="inlineStr">
+      <c r="O3" t="inlineStr">
         <is>
           <t>377</t>
         </is>
       </c>
-      <c r="O3" t="inlineStr">
+      <c r="P3" t="inlineStr">
         <is>
           <t>143340</t>
         </is>
       </c>
-      <c r="P3" t="inlineStr">
+      <c r="Q3" t="inlineStr">
         <is>
           <t>chr1:146340-146717</t>
         </is>
@@ -725,14 +740,19 @@
       </c>
       <c r="K4" t="inlineStr">
         <is>
+          <t>1856075</t>
+        </is>
+      </c>
+      <c r="L4" t="inlineStr">
+        <is>
           <t>ct_16_22</t>
         </is>
       </c>
-      <c r="L4" t="inlineStr"/>
       <c r="M4" t="inlineStr"/>
       <c r="N4" t="inlineStr"/>
       <c r="O4" t="inlineStr"/>
       <c r="P4" t="inlineStr"/>
+      <c r="Q4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -785,12 +805,17 @@
           <t>12489</t>
         </is>
       </c>
-      <c r="K5" t="inlineStr"/>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>47024245</t>
+        </is>
+      </c>
       <c r="L5" t="inlineStr"/>
       <c r="M5" t="inlineStr"/>
       <c r="N5" t="inlineStr"/>
       <c r="O5" t="inlineStr"/>
       <c r="P5" t="inlineStr"/>
+      <c r="Q5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -843,24 +868,29 @@
           <t>110073</t>
         </is>
       </c>
-      <c r="K6" t="inlineStr"/>
+      <c r="K6" t="inlineStr">
+        <is>
+          <t>102921732</t>
+        </is>
+      </c>
       <c r="L6" t="inlineStr"/>
-      <c r="M6" t="inlineStr">
+      <c r="M6" t="inlineStr"/>
+      <c r="N6" t="inlineStr">
         <is>
           <t>FAM157B</t>
         </is>
       </c>
-      <c r="N6" t="inlineStr">
+      <c r="O6" t="inlineStr">
         <is>
           <t>56610</t>
         </is>
       </c>
-      <c r="O6" t="inlineStr">
+      <c r="P6" t="inlineStr">
         <is>
           <t>79421</t>
         </is>
       </c>
-      <c r="P6" t="inlineStr">
+      <c r="Q6" t="inlineStr">
         <is>
           <t>chr9:150478369-150534979</t>
         </is>
@@ -917,24 +947,29 @@
           <t>110073</t>
         </is>
       </c>
-      <c r="K7" t="inlineStr"/>
+      <c r="K7" t="inlineStr">
+        <is>
+          <t>102921732</t>
+        </is>
+      </c>
       <c r="L7" t="inlineStr"/>
-      <c r="M7" t="inlineStr">
+      <c r="M7" t="inlineStr"/>
+      <c r="N7" t="inlineStr">
         <is>
           <t>LOC124902321</t>
         </is>
       </c>
-      <c r="N7" t="inlineStr">
+      <c r="O7" t="inlineStr">
         <is>
           <t>3560</t>
         </is>
       </c>
-      <c r="O7" t="inlineStr">
+      <c r="P7" t="inlineStr">
         <is>
           <t>110553</t>
         </is>
       </c>
-      <c r="P7" t="inlineStr">
+      <c r="Q7" t="inlineStr">
         <is>
           <t>chr9:150500287-150503847</t>
         </is>
@@ -951,7 +986,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P4"/>
+  <dimension ref="A1:Q4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -977,32 +1012,32 @@
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>Crisis-A-11_S11_L001</t>
+          <t>Crisis-A</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>Crisis-B-14_S14_L001</t>
+          <t>Crisis-B</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>Crisis-C-17_S17_L001</t>
+          <t>Crisis-C</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>Pre-A-2_S2_L001</t>
+          <t>Pre-A</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>Pre-B-5_S5_L001</t>
+          <t>Pre-B</t>
         </is>
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
-          <t>Pre-C-8_S8_L001</t>
+          <t>Pre-C</t>
         </is>
       </c>
       <c r="J1" s="1" t="inlineStr">
@@ -1012,30 +1047,35 @@
       </c>
       <c r="K1" s="1" t="inlineStr">
         <is>
-          <t>repeats</t>
+          <t>reg-cen_distance</t>
         </is>
       </c>
       <c r="L1" s="1" t="inlineStr">
         <is>
+          <t>censat_repeats</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
           <t>fragile_sites</t>
         </is>
       </c>
-      <c r="M1" s="1" t="inlineStr">
+      <c r="N1" s="1" t="inlineStr">
         <is>
           <t>genes</t>
         </is>
       </c>
-      <c r="N1" s="1" t="inlineStr">
+      <c r="O1" s="1" t="inlineStr">
         <is>
           <t>gene_lengths</t>
         </is>
       </c>
-      <c r="O1" s="1" t="inlineStr">
+      <c r="P1" s="1" t="inlineStr">
         <is>
           <t>gene-telomere_distances</t>
         </is>
       </c>
-      <c r="P1" s="1" t="inlineStr">
+      <c r="Q1" s="1" t="inlineStr">
         <is>
           <t>gene_positions</t>
         </is>
@@ -1094,14 +1134,19 @@
       </c>
       <c r="K2" t="inlineStr">
         <is>
+          <t>1792071</t>
+        </is>
+      </c>
+      <c r="L2" t="inlineStr">
+        <is>
           <t>ct_16_22</t>
         </is>
       </c>
-      <c r="L2" t="inlineStr"/>
       <c r="M2" t="inlineStr"/>
       <c r="N2" t="inlineStr"/>
       <c r="O2" t="inlineStr"/>
       <c r="P2" t="inlineStr"/>
+      <c r="Q2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -1154,16 +1199,21 @@
           <t>22394247</t>
         </is>
       </c>
-      <c r="K3" t="inlineStr"/>
-      <c r="L3" t="inlineStr">
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>9541782</t>
+        </is>
+      </c>
+      <c r="L3" t="inlineStr"/>
+      <c r="M3" t="inlineStr">
         <is>
           <t>FRA19A</t>
         </is>
       </c>
-      <c r="M3" t="inlineStr"/>
       <c r="N3" t="inlineStr"/>
       <c r="O3" t="inlineStr"/>
       <c r="P3" t="inlineStr"/>
+      <c r="Q3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -1216,24 +1266,29 @@
           <t>37765996</t>
         </is>
       </c>
-      <c r="K4" t="inlineStr"/>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>13804719</t>
+        </is>
+      </c>
       <c r="L4" t="inlineStr"/>
-      <c r="M4" t="inlineStr">
+      <c r="M4" t="inlineStr"/>
+      <c r="N4" t="inlineStr">
         <is>
           <t>GOLGA6L14P</t>
         </is>
       </c>
-      <c r="N4" t="inlineStr">
+      <c r="O4" t="inlineStr">
         <is>
           <t>2925</t>
         </is>
       </c>
-      <c r="O4" t="inlineStr">
+      <c r="P4" t="inlineStr">
         <is>
           <t>37765764</t>
         </is>
       </c>
-      <c r="P4" t="inlineStr">
+      <c r="Q4" t="inlineStr">
         <is>
           <t>chrY:24685111-24688036</t>
         </is>

</xml_diff>